<commit_message>
LP36131, 2025-01-23 11:53: Regel-Commit.
</commit_message>
<xml_diff>
--- a/DMAS.AEC/dmas.xlsx
+++ b/DMAS.AEC/dmas.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balzer\Documents\Projekte\Sulzer\UserStories_Sulzer\DMAS\DMAS.AEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976D8097-4A14-457B-A343-C5C47F39614B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D57C04-F9F3-4E4B-979B-684B488BD63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18660" yWindow="-15240" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{3E5298F4-EF1C-432F-A09B-410E450AC794}"/>
+    <workbookView xWindow="-11025" yWindow="-15630" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{3E5298F4-EF1C-432F-A09B-410E450AC794}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="AoEC Files" sheetId="2" r:id="rId2"/>
-    <sheet name="Tab PRODUCT_COUNTRY_HS92" sheetId="3" r:id="rId3"/>
-    <sheet name="Tab Products" sheetId="4" r:id="rId4"/>
+    <sheet name="Project" sheetId="1" r:id="rId1"/>
+    <sheet name="Budget" sheetId="6" r:id="rId2"/>
+    <sheet name="AoEC Files" sheetId="2" r:id="rId3"/>
+    <sheet name="Tab PRODUCT_COUNTRY_HS92" sheetId="3" r:id="rId4"/>
+    <sheet name="Tabelle5" sheetId="5" r:id="rId5"/>
+    <sheet name="Tab Products" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="92">
   <si>
     <t>DMAS - Meilensteine</t>
   </si>
@@ -288,14 +290,42 @@
   </si>
   <si>
     <t>Tab PRODUCT_COUNTRY_COUNTRY_HS92</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Budget</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>MBASUL200113</t>
+  </si>
+  <si>
+    <t>Bezeichnung</t>
+  </si>
+  <si>
+    <t>CreaDt</t>
+  </si>
+  <si>
+    <t>Dt</t>
+  </si>
+  <si>
+    <t>[$]</t>
+  </si>
+  <si>
+    <t>MBASUL250121</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -378,13 +408,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -414,6 +445,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -753,7 +802,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,6 +917,95 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89679D8-46CC-45FA-8B9C-7BCB4E9F97A6}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="25" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="26"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="24"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="25">
+        <v>45678.63958333333</v>
+      </c>
+      <c r="C8" s="6">
+        <v>45678.63958333333</v>
+      </c>
+      <c r="D8" s="22">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="6">
+        <v>45680.461111111108</v>
+      </c>
+      <c r="D9" s="22">
+        <v>394</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBB8708-1065-49C3-A515-99C0D7D6B067}">
   <dimension ref="A1:D24"/>
   <sheetViews>
@@ -879,16 +1017,16 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="57.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="10"/>
-    <col min="4" max="4" width="18.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="11"/>
+    <col min="4" max="4" width="18.5703125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="6"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -903,15 +1041,15 @@
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>18</v>
       </c>
     </row>
@@ -924,10 +1062,10 @@
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="11">
         <v>189.1</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="9">
         <v>45678.459027777775</v>
       </c>
     </row>
@@ -975,11 +1113,11 @@
       <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="11">
         <f>1400*1024</f>
         <v>1433600</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="9">
         <v>45678.460416666669</v>
       </c>
     </row>
@@ -990,10 +1128,10 @@
       <c r="B18" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="11">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="9">
         <v>45678.463194444441</v>
       </c>
     </row>
@@ -1004,7 +1142,7 @@
       <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="9">
         <v>45678.463194444441</v>
       </c>
     </row>
@@ -1015,7 +1153,7 @@
       <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="9">
         <v>45678.463194444441</v>
       </c>
     </row>
@@ -1026,10 +1164,10 @@
       <c r="B21" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="11">
         <v>0.375</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="9">
         <v>45678.463194444441</v>
       </c>
     </row>
@@ -1040,10 +1178,10 @@
       <c r="B22" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="11">
         <v>0.36499999999999999</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="9">
         <v>45678.463194444441</v>
       </c>
     </row>
@@ -1054,7 +1192,7 @@
       <c r="B23" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="9">
         <v>45678.463194444441</v>
       </c>
     </row>
@@ -1065,7 +1203,7 @@
       <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="9">
         <v>45678.463194444441</v>
       </c>
     </row>
@@ -1077,156 +1215,188 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0074CE0F-5763-4BFB-8F01-2031117045EC}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="11"/>
-    <col min="2" max="2" width="34.85546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="11"/>
-    <col min="4" max="4" width="46" style="13" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="11"/>
+    <col min="1" max="1" width="11.42578125" style="12"/>
+    <col min="2" max="2" width="34.85546875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="12"/>
+    <col min="4" max="4" width="46" style="14" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="F5" s="12" t="str">
+        <f>UPPER(A6)&amp;"      "&amp;LOWER(C6)&amp;","</f>
+        <v>PARTNER_COUNTRY_ID      integer,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="F6" s="12" t="str">
+        <f t="shared" ref="F6:F13" si="0">UPPER(A7)&amp;"      "&amp;LOWER(C7)&amp;","</f>
+        <v>PRODUCT_ID      integer,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="F7" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>YEAR      integer,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="14" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="F8" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>EXPORT_VALUE      integer,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="F9" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>IMPORT_VALUE      integer,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="F10" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>ECI      float,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="F11" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>COI      float,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="F12" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>PCI      float,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1235,12 +1405,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B970C6DB-62A5-4BF7-B63C-7F9B7FDA8289}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E4062D-0CA4-46E2-8F7B-9239BC4F26C1}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,19 +1430,21 @@
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="4" max="4" width="46.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>61</v>
       </c>
@@ -1273,129 +1457,180 @@
       <c r="D5" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="13" t="s">
         <v>70</v>
       </c>
       <c r="C6" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="12"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="13"/>
+      <c r="E6" t="str">
+        <f>A6&amp;"      "&amp;LOWER(C6)&amp;","</f>
+        <v>product_id      integer,</v>
+      </c>
+      <c r="F6" t="str">
+        <f>UPPER(A6)&amp;"      "&amp;LOWER(C6)&amp;","</f>
+        <v>PRODUCT_ID      integer,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="13"/>
+      <c r="E7" t="str">
+        <f t="shared" ref="E7:E11" si="0">A7&amp;"      "&amp;LOWER(C7)&amp;","</f>
+        <v>code      string,</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" ref="F7:F11" si="1">UPPER(A7)&amp;"      "&amp;LOWER(C7)&amp;","</f>
+        <v>CODE      string,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="13" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>name_short_en      string,</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>NAME_SHORT_EN      string,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="13" t="s">
         <v>73</v>
       </c>
       <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>product_level      integer,</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>PRODUCT_LEVEL      integer,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>74</v>
       </c>
       <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="13"/>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>top_parent_id      integer,</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>TOP_PARENT_ID      integer,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="13" t="s">
         <v>75</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" spans="1:4" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>product_id_hierarchy      string,</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>PRODUCT_ID_HIERARCHY      string,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="13"/>
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="D13" s="17"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="18"/>
+      <c r="D13" s="18"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="13" t="s">
         <v>70</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>76</v>
       </c>
       <c r="C15" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="13" t="s">
         <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="13" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1403,13 +1638,13 @@
       <c r="A17" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="13" t="s">
         <v>73</v>
       </c>
       <c r="C17" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="13" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1417,13 +1652,13 @@
       <c r="A18" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="13" t="s">
         <v>80</v>
       </c>
       <c r="C18" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="12"/>
+      <c r="D18" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LP36131: Notebook draft, Doku-Skizzen.
</commit_message>
<xml_diff>
--- a/DMAS.AEC/dmas.xlsx
+++ b/DMAS.AEC/dmas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balzer\Documents\Projekte\Sulzer\UserStories_Sulzer\DMAS\DMAS.AEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B2A8A7-5047-428C-BDA9-3486CEC424B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FC76E7-538B-4724-9C89-46283DE49B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3E5298F4-EF1C-432F-A09B-410E450AC794}"/>
+    <workbookView xWindow="15210" yWindow="-15870" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{3E5298F4-EF1C-432F-A09B-410E450AC794}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="161">
   <si>
     <t>DMAS - Meilensteine</t>
   </si>
@@ -663,6 +663,30 @@
   </si>
   <si>
     <t xml:space="preserve">Explizites Erstellen der Zieltabelle für jede Quelldatei erforderlich (RAW_...) </t>
+  </si>
+  <si>
+    <t>Benchmark für hs12_country_product_year_2</t>
+  </si>
+  <si>
+    <t>Kosten</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
+  </si>
+  <si>
+    <t>Stage, intern</t>
+  </si>
+  <si>
+    <t>Upload</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
+  <si>
+    <t>Gesamt</t>
+  </si>
+  <si>
+    <t>Dauer [sec]</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1055,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1199,6 +1223,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1658,7 +1688,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2358,13 +2388,22 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E37" s="20" t="str">
+      <c r="A37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="6">
+        <v>45736.772916666669</v>
+      </c>
+      <c r="D37" s="15">
+        <v>288</v>
+      </c>
+      <c r="E37" s="20">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="F37" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="F37" s="20">
         <f t="shared" si="4"/>
-        <v/>
+        <v>-36</v>
       </c>
       <c r="G37" s="20" t="str">
         <f t="shared" si="5"/>
@@ -2984,10 +3023,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F8BBA-8806-41EF-8979-2B592A349284}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3411,6 +3453,9 @@
       <c r="H28" s="62"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>153</v>
+      </c>
       <c r="C29" s="45"/>
       <c r="D29" s="61"/>
       <c r="E29" s="62"/>
@@ -3419,6 +3464,12 @@
       <c r="H29" s="62"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="72" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>157</v>
+      </c>
       <c r="C30" s="45"/>
       <c r="D30" s="61"/>
       <c r="E30" s="62"/>
@@ -3427,6 +3478,10 @@
       <c r="H30" s="62"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="72"/>
+      <c r="B31" s="31" t="s">
+        <v>158</v>
+      </c>
       <c r="C31" s="45"/>
       <c r="D31" s="61"/>
       <c r="E31" s="62"/>
@@ -3435,6 +3490,10 @@
       <c r="H31" s="62"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="72"/>
+      <c r="B32" s="31" t="s">
+        <v>159</v>
+      </c>
       <c r="C32" s="45"/>
       <c r="D32" s="61"/>
       <c r="E32" s="62"/>
@@ -3442,9 +3501,37 @@
       <c r="G32" s="62"/>
       <c r="H32" s="62"/>
     </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="73" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="45"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="62"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="73"/>
+      <c r="B34" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="45"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="D3:H3"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LP36131: Dataload mit SQLAlchemy.
</commit_message>
<xml_diff>
--- a/DMAS.AEC/dmas.xlsx
+++ b/DMAS.AEC/dmas.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balzer\Documents\Projekte\Sulzer\UserStories_Sulzer\DMAS\DMAS.AEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FC76E7-538B-4724-9C89-46283DE49B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0030F68E-121E-43D5-B194-EAC61D161B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15210" yWindow="-15870" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{3E5298F4-EF1C-432F-A09B-410E450AC794}"/>
+    <workbookView xWindow="-9870" yWindow="-14055" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{3E5298F4-EF1C-432F-A09B-410E450AC794}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
     <sheet name="Budget" sheetId="6" r:id="rId2"/>
-    <sheet name="AoEC Files" sheetId="2" r:id="rId3"/>
-    <sheet name="AoEC-Dateien" sheetId="11" r:id="rId4"/>
-    <sheet name="Ladeverfahren" sheetId="12" r:id="rId5"/>
-    <sheet name="Prod.vergleiche" sheetId="7" r:id="rId6"/>
-    <sheet name="Tab-Cols CCPY" sheetId="9" r:id="rId7"/>
-    <sheet name="Tableau-Dta" sheetId="10" r:id="rId8"/>
+    <sheet name="Benchmark" sheetId="13" r:id="rId3"/>
+    <sheet name="AoEC Files" sheetId="2" r:id="rId4"/>
+    <sheet name="AoEC-Dateien" sheetId="11" r:id="rId5"/>
+    <sheet name="Ladeverfahren" sheetId="12" r:id="rId6"/>
+    <sheet name="Prod.vergleiche" sheetId="7" r:id="rId7"/>
+    <sheet name="Tab-Cols CCPY" sheetId="9" r:id="rId8"/>
+    <sheet name="Tableau-Dta" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="181">
   <si>
     <t>DMAS - Meilensteine</t>
   </si>
@@ -688,6 +689,87 @@
   <si>
     <t>Dauer [sec]</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>Æ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> [$/d]</t>
+    </r>
+  </si>
+  <si>
+    <t>Benchmarks</t>
+  </si>
+  <si>
+    <t>Verfahren</t>
+  </si>
+  <si>
+    <t>Src</t>
+  </si>
+  <si>
+    <t>Trg</t>
+  </si>
+  <si>
+    <t>[mi:ss]</t>
+  </si>
+  <si>
+    <t>[sec]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COPY </t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Python, SQLAlchemy</t>
+  </si>
+  <si>
+    <t>Notebook, SQLAlchemy</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Ausführung</t>
+  </si>
+  <si>
+    <t>#Rows</t>
+  </si>
+  <si>
+    <t>40:07</t>
+  </si>
+  <si>
+    <t>43:35</t>
+  </si>
+  <si>
+    <t>Chunksize</t>
+  </si>
+  <si>
+    <t>Warehouse [Cred/h]</t>
+  </si>
+  <si>
+    <t>39:11</t>
+  </si>
 </sst>
 </file>
 
@@ -699,7 +781,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -838,6 +920,47 @@
       <name val="Aptos Narrow"/>
       <family val="1"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1055,7 +1178,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1212,6 +1335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1228,6 +1352,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1687,8 +1847,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89679D8-46CC-45FA-8B9C-7BCB4E9F97A6}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1705,14 +1866,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68" t="s">
+      <c r="B3" s="69"/>
+      <c r="C3" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="68"/>
+      <c r="D3" s="69"/>
       <c r="E3" s="12" t="s">
         <v>38</v>
       </c>
@@ -1735,6 +1896,9 @@
       </c>
       <c r="F4" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="G4" s="68" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2411,45 +2575,72 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E38" s="20" t="str">
+      <c r="A38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="6">
+        <v>45740.453472222223</v>
+      </c>
+      <c r="D38" s="15">
+        <v>273</v>
+      </c>
+      <c r="E38" s="20">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="F38" s="20" t="str">
+        <v>4</v>
+      </c>
+      <c r="F38" s="20">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="G38" s="20" t="str">
+        <v>-15</v>
+      </c>
+      <c r="G38" s="20">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-3.75</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E39" s="20" t="str">
+      <c r="A39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="6">
+        <v>45741.414583333331</v>
+      </c>
+      <c r="D39" s="15">
+        <v>258</v>
+      </c>
+      <c r="E39" s="20">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="F39" s="20" t="str">
+        <v>1</v>
+      </c>
+      <c r="F39" s="20">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="G39" s="20" t="str">
+        <v>-15</v>
+      </c>
+      <c r="G39" s="20">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-15</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E40" s="20" t="str">
+      <c r="A40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="6">
+        <v>45742.443749999999</v>
+      </c>
+      <c r="D40" s="15">
+        <v>241</v>
+      </c>
+      <c r="E40" s="20">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="F40" s="20" t="str">
+        <v>1</v>
+      </c>
+      <c r="F40" s="20">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="G40" s="20" t="str">
+        <v>-17</v>
+      </c>
+      <c r="G40" s="20">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-17</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2490,6 +2681,211 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C41FD51-0CA1-4573-936F-5B7AC947B626}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="30"/>
+    <col min="4" max="4" width="11.28515625" style="77" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="77" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="77" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="83"/>
+    <col min="8" max="9" width="11.42578125" style="80"/>
+    <col min="10" max="16384" width="11.42578125" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="43" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="75" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="81"/>
+    </row>
+    <row r="5" spans="1:9" s="38" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" s="76" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5" s="76" t="s">
+        <v>178</v>
+      </c>
+      <c r="F5" s="79" t="s">
+        <v>174</v>
+      </c>
+      <c r="G5" s="85" t="s">
+        <v>166</v>
+      </c>
+      <c r="H5" s="86" t="s">
+        <v>167</v>
+      </c>
+      <c r="I5" s="86" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="77">
+        <v>1</v>
+      </c>
+      <c r="E10" s="77">
+        <v>20000</v>
+      </c>
+      <c r="F10" s="78">
+        <v>45741.670138888891</v>
+      </c>
+      <c r="G10" s="83" t="s">
+        <v>176</v>
+      </c>
+      <c r="H10" s="80">
+        <f>40*60+7</f>
+        <v>2407</v>
+      </c>
+      <c r="I10" s="80">
+        <v>5578124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="77">
+        <v>1</v>
+      </c>
+      <c r="E11" s="77">
+        <v>100000</v>
+      </c>
+      <c r="F11" s="78">
+        <v>45741.841666666667</v>
+      </c>
+      <c r="G11" s="83" t="s">
+        <v>177</v>
+      </c>
+      <c r="H11" s="80">
+        <f>43*60+35</f>
+        <v>2615</v>
+      </c>
+      <c r="I11" s="80">
+        <v>5578124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="77">
+        <v>4</v>
+      </c>
+      <c r="E12" s="77">
+        <v>20000</v>
+      </c>
+      <c r="F12" s="78">
+        <v>45742.740277777775</v>
+      </c>
+      <c r="G12" s="83" t="s">
+        <v>180</v>
+      </c>
+      <c r="H12" s="80">
+        <v>2351</v>
+      </c>
+      <c r="I12" s="80">
+        <v>5578124</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="D4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBB8708-1065-49C3-A515-99C0D7D6B067}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -2847,7 +3243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DA5C6D-7D2B-4A79-97CE-CC25C1EABB3F}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -3021,7 +3417,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F8BBA-8806-41EF-8979-2B592A349284}">
   <dimension ref="A1:H34"/>
   <sheetViews>
@@ -3050,13 +3446,13 @@
     <row r="3" spans="1:8" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="40"/>
       <c r="C3" s="41"/>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="72"/>
     </row>
     <row r="4" spans="1:8" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
@@ -3464,7 +3860,7 @@
       <c r="H29" s="62"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="72" t="s">
+      <c r="A30" s="73" t="s">
         <v>160</v>
       </c>
       <c r="B30" s="31" t="s">
@@ -3478,7 +3874,7 @@
       <c r="H30" s="62"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="72"/>
+      <c r="A31" s="73"/>
       <c r="B31" s="31" t="s">
         <v>158</v>
       </c>
@@ -3490,7 +3886,7 @@
       <c r="H31" s="62"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="72"/>
+      <c r="A32" s="73"/>
       <c r="B32" s="31" t="s">
         <v>159</v>
       </c>
@@ -3502,7 +3898,7 @@
       <c r="H32" s="62"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="73" t="s">
+      <c r="A33" s="74" t="s">
         <v>154</v>
       </c>
       <c r="B33" s="31" t="s">
@@ -3516,7 +3912,7 @@
       <c r="H33" s="62"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="73"/>
+      <c r="A34" s="74"/>
       <c r="B34" s="31" t="s">
         <v>156</v>
       </c>
@@ -3537,7 +3933,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7BE676B-1D24-4249-BF84-885166B1803C}">
   <dimension ref="A1:I8"/>
   <sheetViews>
@@ -3597,7 +3993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67D15E6-538C-4C71-B986-1FBD2827D701}">
   <dimension ref="A1:T8"/>
   <sheetViews>
@@ -4019,7 +4415,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55FCAF5-7C9D-447F-A170-5465EBE0C70D}">
   <dimension ref="A1:C15"/>
   <sheetViews>

</xml_diff>

<commit_message>
LP36131: vor Einführung von Notebook IMPORT_HS12_INTERNAL_STAGE_STATA_3 in Github.
</commit_message>
<xml_diff>
--- a/DMAS.AEC/dmas.xlsx
+++ b/DMAS.AEC/dmas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balzer\Documents\Projekte\Sulzer\UserStories_Sulzer\DMAS\DMAS.AEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0030F68E-121E-43D5-B194-EAC61D161B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8141B46-4E1E-4ACF-942C-910C3BEF0D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9870" yWindow="-14055" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{3E5298F4-EF1C-432F-A09B-410E450AC794}"/>
+    <workbookView xWindow="-13590" yWindow="-16395" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3E5298F4-EF1C-432F-A09B-410E450AC794}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="181">
   <si>
     <t>DMAS - Meilensteine</t>
   </si>
@@ -1336,9 +1336,45 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1352,42 +1388,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1847,9 +1847,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89679D8-46CC-45FA-8B9C-7BCB4E9F97A6}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
+      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1866,14 +1866,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69" t="s">
+      <c r="B3" s="80"/>
+      <c r="C3" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="69"/>
+      <c r="D3" s="80"/>
       <c r="E3" s="12" t="s">
         <v>38</v>
       </c>
@@ -2644,9 +2644,15 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E41" s="20" t="str">
+      <c r="A41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="6">
+        <v>45743.451388888891</v>
+      </c>
+      <c r="E41" s="20">
         <f t="shared" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="F41" s="20" t="str">
         <f t="shared" si="4"/>
@@ -2658,9 +2664,18 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E42" s="20" t="str">
+      <c r="A42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="6">
+        <v>45745.740972222222</v>
+      </c>
+      <c r="D42" s="15">
+        <v>227</v>
+      </c>
+      <c r="E42" s="20">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="F42" s="20" t="str">
         <f t="shared" si="4"/>
@@ -2684,19 +2699,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C41FD51-0CA1-4573-936F-5B7AC947B626}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" style="30" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.42578125" style="30"/>
-    <col min="4" max="4" width="11.28515625" style="77" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="77" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="77" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="83"/>
-    <col min="8" max="9" width="11.42578125" style="80"/>
+    <col min="4" max="4" width="11.28515625" style="70" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="70" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="76"/>
+    <col min="8" max="9" width="11.42578125" style="73"/>
     <col min="10" max="16384" width="11.42578125" style="30"/>
   </cols>
   <sheetData>
@@ -2706,16 +2721,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="43" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="81" t="s">
         <v>173</v>
       </c>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75" t="s">
+      <c r="E4" s="81"/>
+      <c r="F4" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="74"/>
     </row>
     <row r="5" spans="1:9" s="38" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
@@ -2727,32 +2742,32 @@
       <c r="C5" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="69" t="s">
         <v>179</v>
       </c>
-      <c r="E5" s="76" t="s">
+      <c r="E5" s="69" t="s">
         <v>178</v>
       </c>
-      <c r="F5" s="79" t="s">
+      <c r="F5" s="72" t="s">
         <v>174</v>
       </c>
-      <c r="G5" s="85" t="s">
+      <c r="G5" s="78" t="s">
         <v>166</v>
       </c>
-      <c r="H5" s="86" t="s">
+      <c r="H5" s="79" t="s">
         <v>167</v>
       </c>
-      <c r="I5" s="86" t="s">
+      <c r="I5" s="79" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
@@ -2797,23 +2812,23 @@
       <c r="C10" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="D10" s="77">
+      <c r="D10" s="70">
         <v>1</v>
       </c>
-      <c r="E10" s="77">
+      <c r="E10" s="70">
         <v>20000</v>
       </c>
-      <c r="F10" s="78">
+      <c r="F10" s="71">
         <v>45741.670138888891</v>
       </c>
-      <c r="G10" s="83" t="s">
+      <c r="G10" s="76" t="s">
         <v>176</v>
       </c>
-      <c r="H10" s="80">
+      <c r="H10" s="73">
         <f>40*60+7</f>
         <v>2407</v>
       </c>
-      <c r="I10" s="80">
+      <c r="I10" s="73">
         <v>5578124</v>
       </c>
     </row>
@@ -2827,23 +2842,23 @@
       <c r="C11" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="D11" s="77">
+      <c r="D11" s="70">
         <v>1</v>
       </c>
-      <c r="E11" s="77">
+      <c r="E11" s="70">
         <v>100000</v>
       </c>
-      <c r="F11" s="78">
+      <c r="F11" s="71">
         <v>45741.841666666667</v>
       </c>
-      <c r="G11" s="83" t="s">
+      <c r="G11" s="76" t="s">
         <v>177</v>
       </c>
-      <c r="H11" s="80">
+      <c r="H11" s="73">
         <f>43*60+35</f>
         <v>2615</v>
       </c>
-      <c r="I11" s="80">
+      <c r="I11" s="73">
         <v>5578124</v>
       </c>
     </row>
@@ -2857,22 +2872,22 @@
       <c r="C12" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="D12" s="77">
+      <c r="D12" s="70">
         <v>4</v>
       </c>
-      <c r="E12" s="77">
+      <c r="E12" s="70">
         <v>20000</v>
       </c>
-      <c r="F12" s="78">
+      <c r="F12" s="71">
         <v>45742.740277777775</v>
       </c>
-      <c r="G12" s="83" t="s">
+      <c r="G12" s="76" t="s">
         <v>180</v>
       </c>
-      <c r="H12" s="80">
+      <c r="H12" s="73">
         <v>2351</v>
       </c>
-      <c r="I12" s="80">
+      <c r="I12" s="73">
         <v>5578124</v>
       </c>
     </row>
@@ -3446,13 +3461,13 @@
     <row r="3" spans="1:8" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="40"/>
       <c r="C3" s="41"/>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="72"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="84"/>
     </row>
     <row r="4" spans="1:8" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
@@ -3860,7 +3875,7 @@
       <c r="H29" s="62"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="73" t="s">
+      <c r="A30" s="85" t="s">
         <v>160</v>
       </c>
       <c r="B30" s="31" t="s">
@@ -3874,7 +3889,7 @@
       <c r="H30" s="62"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="73"/>
+      <c r="A31" s="85"/>
       <c r="B31" s="31" t="s">
         <v>158</v>
       </c>
@@ -3886,7 +3901,7 @@
       <c r="H31" s="62"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="73"/>
+      <c r="A32" s="85"/>
       <c r="B32" s="31" t="s">
         <v>159</v>
       </c>
@@ -3898,7 +3913,7 @@
       <c r="H32" s="62"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="74" t="s">
+      <c r="A33" s="86" t="s">
         <v>154</v>
       </c>
       <c r="B33" s="31" t="s">
@@ -3912,7 +3927,7 @@
       <c r="H33" s="62"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="74"/>
+      <c r="A34" s="86"/>
       <c r="B34" s="31" t="s">
         <v>156</v>
       </c>

</xml_diff>